<commit_message>
remake tables and other predictions
</commit_message>
<xml_diff>
--- a/output/table/prediction_accuracy.xlsx
+++ b/output/table/prediction_accuracy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yujunzhou/Box Sync/Research/WD-Early-Warning-Food-Insecurity/output/table/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\WD-Early-Warning-Food-Insecurity\output\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6DA5B48-F3AF-9544-85EE-9699CD470C57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D0C521-FF41-45E9-84CA-B82DF847E9F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16140" xr2:uid="{EF8B5D74-F3EE-6047-970C-FF2D548912EC}"/>
+    <workbookView xWindow="14400" yWindow="465" windowWidth="14400" windowHeight="16140" xr2:uid="{EF8B5D74-F3EE-6047-970C-FF2D548912EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>random.ols</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>rCSI</t>
+  </si>
+  <si>
+    <t>year.ols+ quarterFE</t>
+  </si>
+  <si>
+    <t>year.ols+ monthFE+quaterFE</t>
+  </si>
+  <si>
+    <t>random.ols+ quarterFE</t>
+  </si>
+  <si>
+    <t>random.ols+ monthFE+quaterFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old result </t>
   </si>
 </sst>
 </file>
@@ -53,9 +68,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,7 +101,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,18 +416,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739AA721-BBF2-6148-BB0D-9BD7EF1061B4}">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="2" max="2" width="31.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -423,63 +438,144 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="D3">
+        <v>0.623</v>
+      </c>
+      <c r="E3">
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.54527760000000003</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.61605690000000002</v>
-      </c>
-      <c r="E3" s="1">
-        <v>8.1974870000000005E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" t="s">
+      <c r="C5" s="1">
+        <v>0.54870490000000005</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.56888430000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.1299255</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.55995499999999998</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.60089119999999996</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.1272171</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.56921231000000005</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.59517779999999998</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.1001644</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.54483309999999996</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.60430329999999999</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7.9707260000000002E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" t="s">
+      <c r="C8" s="1">
+        <v>0.56968423999999995</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.60020070000000003</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.11101</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.50394329999999998</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.50394329999999998</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.18707190000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" t="s">
+      <c r="C11" s="1">
+        <v>0.49707180000000001</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.5477649</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9.5098600000000005E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.51814559999999998</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.54071519999999995</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.1117934</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.52620599999999995</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.54198760000000001</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.1802338</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.50993049999999995</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.52244979999999996</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.23074210000000001</v>
+      <c r="C14" s="1">
+        <v>0.50783639999999997</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.5592047</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.1662719</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
lag price and region fixed effect
</commit_message>
<xml_diff>
--- a/output/table/prediction_accuracy.xlsx
+++ b/output/table/prediction_accuracy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\WD-Early-Warning-Food-Insecurity\output\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D0C521-FF41-45E9-84CA-B82DF847E9F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CEBF63-EC66-452D-8EDC-CF41EEB4A4A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="465" windowWidth="14400" windowHeight="16140" xr2:uid="{EF8B5D74-F3EE-6047-970C-FF2D548912EC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>random.ols</t>
   </si>
@@ -51,9 +51,6 @@
     <t>year.ols+ quarterFE</t>
   </si>
   <si>
-    <t>year.ols+ monthFE+quaterFE</t>
-  </si>
-  <si>
     <t>random.ols+ quarterFE</t>
   </si>
   <si>
@@ -61,6 +58,27 @@
   </si>
   <si>
     <t xml:space="preserve">Old result </t>
+  </si>
+  <si>
+    <t>R squared</t>
+  </si>
+  <si>
+    <t>Predicting insecure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall accuracy </t>
+  </si>
+  <si>
+    <t>year.ols+quarter*region FE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year.ols+ monthFE </t>
+  </si>
+  <si>
+    <t>year.ols + lag price</t>
+  </si>
+  <si>
+    <t>year.ols + GIEWS price</t>
   </si>
 </sst>
 </file>
@@ -99,9 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739AA721-BBF2-6148-BB0D-9BD7EF1061B4}">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -427,7 +448,24 @@
     <col min="2" max="2" width="31.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -437,10 +475,28 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>0.53600000000000003</v>
@@ -452,7 +508,7 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -466,115 +522,149 @@
         <v>0.1299255</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C9" s="1">
         <v>0.55995499999999998</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D9" s="1">
         <v>0.60089119999999996</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E9" s="1">
         <v>0.1272171</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.56921231000000005</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.59517779999999998</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.1001644</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.56968423999999995</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.60020070000000003</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.11101</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.49707180000000001</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.5477649</v>
+      </c>
+      <c r="E32" s="1">
+        <v>9.5098600000000005E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.56921231000000005</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.59517779999999998</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.1001644</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.56968423999999995</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.60020070000000003</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.11101</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.49707180000000001</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.5477649</v>
-      </c>
-      <c r="E11" s="1">
-        <v>9.5098600000000005E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="C33" s="1">
+        <v>0.51814559999999998</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.54071519999999995</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.1117934</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.51814559999999998</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.54071519999999995</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.1117934</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="C34" s="1">
         <v>0.52620599999999995</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D34" s="1">
         <v>0.54198760000000001</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E34" s="1">
         <v>0.1802338</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C35" s="1">
         <v>0.50783639999999997</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D35" s="1">
         <v>0.5592047</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E35" s="1">
         <v>0.1662719</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>